<commit_message>
updated files for the new run
</commit_message>
<xml_diff>
--- a/books/carbomica_databook.xlsx
+++ b/books/carbomica_databook.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="31">
   <si>
     <t>Abbreviation</t>
   </si>
@@ -51,10 +51,10 @@
     <t>Population type</t>
   </si>
   <si>
-    <t>mt_darwin</t>
-  </si>
-  <si>
-    <t>Mt Darwin</t>
+    <t>mb_hosp</t>
+  </si>
+  <si>
+    <t>Mombasa Hospital</t>
   </si>
   <si>
     <t>facilities</t>
@@ -87,18 +87,21 @@
     <t>N.A.</t>
   </si>
   <si>
-    <t>Vehicle Fuel - baseline</t>
-  </si>
-  <si>
-    <t>Travel - baseline</t>
+    <t>Bottled gas(LPG) - baseline</t>
+  </si>
+  <si>
+    <t>Refridgerants - baseline</t>
+  </si>
+  <si>
+    <t>Liquid fuel(Petrol or Diesel) - baseline</t>
+  </si>
+  <si>
+    <t>Vehicle Fuel (Owned Vehicles) - baseline</t>
   </si>
   <si>
     <t>Anaesthetic Gases - baseline</t>
   </si>
   <si>
-    <t>Refridgerant - baseline</t>
-  </si>
-  <si>
     <t>Waste - baseline</t>
   </si>
   <si>
@@ -111,16 +114,19 @@
     <t>Framework-supplied default</t>
   </si>
   <si>
-    <t>Vehicle Fuel - multiplier</t>
-  </si>
-  <si>
-    <t>Travel - multiplier</t>
+    <t>Bottled gas(LPG) - multiplier</t>
+  </si>
+  <si>
+    <t>Refridgerants - multiplier</t>
+  </si>
+  <si>
+    <t>Liquid fuel(Petrol or Diesel) - multiplier</t>
+  </si>
+  <si>
+    <t>Vehicle Fuel (Owned Vehicles) - multiplier</t>
   </si>
   <si>
     <t>Anaesthetic Gases - multiplier</t>
-  </si>
-  <si>
-    <t>Refridgerant - multiplier</t>
   </si>
   <si>
     <t>Waste - multiplier</t>
@@ -547,7 +553,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -622,7 +628,7 @@
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
-        <v>mt_darwin</v>
+        <v>mb_hosp</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -660,13 +666,13 @@
   <sheetPr>
     <tabColor rgb="FF808080"/>
   </sheetPr>
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="32.5703125" customWidth="1"/>
+    <col min="1" max="1" width="45.7109375" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="7.28515625" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" customWidth="1"/>
@@ -699,7 +705,7 @@
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
-        <v>mt_darwin</v>
+        <v>mb_hosp</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -710,7 +716,7 @@
         <v>12</v>
       </c>
       <c r="G2" s="3">
-        <v>39.73</v>
+        <v>17.13</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -737,7 +743,7 @@
     <row r="5" spans="1:7">
       <c r="A5" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
-        <v>mt_darwin</v>
+        <v>mb_hosp</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
@@ -748,7 +754,7 @@
         <v>12</v>
       </c>
       <c r="G5" s="3">
-        <v>27.76</v>
+        <v>27.42</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -775,7 +781,7 @@
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
-        <v>mt_darwin</v>
+        <v>mb_hosp</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
@@ -786,7 +792,7 @@
         <v>12</v>
       </c>
       <c r="G8" s="3">
-        <v>0.12</v>
+        <v>107.27</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -813,7 +819,7 @@
     <row r="11" spans="1:7">
       <c r="A11" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
-        <v>mt_darwin</v>
+        <v>mb_hosp</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
@@ -824,7 +830,7 @@
         <v>12</v>
       </c>
       <c r="G11" s="3">
-        <v>3.05</v>
+        <v>69.45</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -851,7 +857,7 @@
     <row r="14" spans="1:7">
       <c r="A14" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
-        <v>mt_darwin</v>
+        <v>mb_hosp</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
@@ -862,7 +868,7 @@
         <v>12</v>
       </c>
       <c r="G14" s="3">
-        <v>0</v>
+        <v>259.15</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -889,7 +895,7 @@
     <row r="17" spans="1:7">
       <c r="A17" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
-        <v>mt_darwin</v>
+        <v>mb_hosp</v>
       </c>
       <c r="C17" t="s">
         <v>14</v>
@@ -900,7 +906,7 @@
         <v>12</v>
       </c>
       <c r="G17" s="3">
-        <v>2.28</v>
+        <v>420.18</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -927,7 +933,7 @@
     <row r="20" spans="1:7">
       <c r="A20" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
-        <v>mt_darwin</v>
+        <v>mb_hosp</v>
       </c>
       <c r="C20" t="s">
         <v>14</v>
@@ -938,7 +944,45 @@
         <v>12</v>
       </c>
       <c r="G20" s="3">
-        <v>2.34</v>
+        <v>582.86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="1" t="str">
+        <f>'Population Definitions'!$A$2</f>
+        <v>mb_hosp</v>
+      </c>
+      <c r="C23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="3">
+        <v>720.24</v>
       </c>
     </row>
   </sheetData>
@@ -982,6 +1026,14 @@
       <formula>AND(COUNTIF(G20:G20,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E20)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E23">
+    <cfRule type="expression" dxfId="0" priority="15">
+      <formula>COUNTIF(G23:G23,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="16">
+      <formula>AND(COUNTIF(G23:G23,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E23)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="E5">
     <cfRule type="expression" dxfId="0" priority="3">
       <formula>COUNTIF(G5:G5,"&lt;&gt;" &amp; "")&gt;0</formula>
@@ -998,7 +1050,7 @@
       <formula>AND(COUNTIF(G8:G8,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E8)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="7">
+  <dataValidations count="8">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2">
       <formula1>"N.A."</formula1>
     </dataValidation>
@@ -1018,6 +1070,9 @@
       <formula1>"N.A."</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C20">
+      <formula1>"N.A."</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C23">
       <formula1>"N.A."</formula1>
     </dataValidation>
   </dataValidations>
@@ -1030,13 +1085,13 @@
   <sheetPr>
     <tabColor rgb="FF808080"/>
   </sheetPr>
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" customWidth="1"/>
+    <col min="1" max="1" width="47.85546875" customWidth="1"/>
     <col min="2" max="2" width="30.28515625" customWidth="1"/>
     <col min="3" max="3" width="7.28515625" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" customWidth="1"/>
@@ -1047,7 +1102,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>7</v>
@@ -1069,10 +1124,10 @@
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
-        <v>mt_darwin</v>
+        <v>mb_hosp</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -1088,7 +1143,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
@@ -1110,10 +1165,10 @@
     <row r="5" spans="1:7">
       <c r="A5" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
-        <v>mt_darwin</v>
+        <v>mb_hosp</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
@@ -1129,7 +1184,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>7</v>
@@ -1151,10 +1206,10 @@
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
-        <v>mt_darwin</v>
+        <v>mb_hosp</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
@@ -1170,7 +1225,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>7</v>
@@ -1192,10 +1247,10 @@
     <row r="11" spans="1:7">
       <c r="A11" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
-        <v>mt_darwin</v>
+        <v>mb_hosp</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
@@ -1211,7 +1266,7 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
@@ -1233,10 +1288,10 @@
     <row r="14" spans="1:7">
       <c r="A14" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
-        <v>mt_darwin</v>
+        <v>mb_hosp</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
@@ -1252,7 +1307,7 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>7</v>
@@ -1274,10 +1329,10 @@
     <row r="17" spans="1:7">
       <c r="A17" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
-        <v>mt_darwin</v>
+        <v>mb_hosp</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
         <v>14</v>
@@ -1293,7 +1348,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>7</v>
@@ -1315,10 +1370,10 @@
     <row r="20" spans="1:7">
       <c r="A20" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
-        <v>mt_darwin</v>
+        <v>mb_hosp</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
         <v>14</v>
@@ -1331,6 +1386,47 @@
         <v>12</v>
       </c>
       <c r="G20" s="3"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="1" t="str">
+        <f>'Population Definitions'!$A$2</f>
+        <v>mb_hosp</v>
+      </c>
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3">
+        <v>0</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E11">
@@ -1373,6 +1469,14 @@
       <formula>AND(COUNTIF(G20:G20,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E20)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E23">
+    <cfRule type="expression" dxfId="0" priority="15">
+      <formula>COUNTIF(G23:G23,"&lt;&gt;" &amp; "")&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="16">
+      <formula>AND(COUNTIF(G23:G23,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E23)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="E5">
     <cfRule type="expression" dxfId="0" priority="3">
       <formula>COUNTIF(G5:G5,"&lt;&gt;" &amp; "")&gt;0</formula>
@@ -1389,7 +1493,7 @@
       <formula>AND(COUNTIF(G8:G8,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E8)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="7">
+  <dataValidations count="8">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2">
       <formula1>"N.A."</formula1>
     </dataValidation>
@@ -1409,6 +1513,9 @@
       <formula1>"N.A."</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C20">
+      <formula1>"N.A."</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C23">
       <formula1>"N.A."</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
updated sim timeframe and input data sheet
</commit_message>
<xml_diff>
--- a/books/carbomica_databook.xlsx
+++ b/books/carbomica_databook.xlsx
@@ -589,7 +589,7 @@
   <sheetPr>
     <tabColor rgb="FF808080"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -602,9 +602,13 @@
     <col min="5" max="5" width="10.5703125" customWidth="1"/>
     <col min="6" max="6" width="3.85546875" customWidth="1"/>
     <col min="7" max="7" width="9.42578125" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -622,10 +626,22 @@
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>2024</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2025</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2026</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2027</v>
+      </c>
+      <c r="K1" s="1">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>AKHS_Mombasa</v>
@@ -641,14 +657,18 @@
       <c r="G2" s="3">
         <v>1</v>
       </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>COUNTIF(G2:G2,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(G2:K2,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="2">
-      <formula>AND(COUNTIF(G2:G2,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E2)))</formula>
+      <formula>AND(COUNTIF(G2:K2,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -666,7 +686,7 @@
   <sheetPr>
     <tabColor rgb="FF808080"/>
   </sheetPr>
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -679,9 +699,13 @@
     <col min="5" max="5" width="10.5703125" customWidth="1"/>
     <col min="6" max="6" width="3.85546875" customWidth="1"/>
     <col min="7" max="7" width="9.42578125" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -699,10 +723,22 @@
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>2024</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2025</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2026</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2027</v>
+      </c>
+      <c r="K1" s="1">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>AKHS_Mombasa</v>
@@ -718,8 +754,12 @@
       <c r="G2" s="3">
         <v>109530.344</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -737,10 +777,22 @@
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>2024</v>
+      </c>
+      <c r="H4" s="1">
+        <v>2025</v>
+      </c>
+      <c r="I4" s="1">
+        <v>2026</v>
+      </c>
+      <c r="J4" s="1">
+        <v>2027</v>
+      </c>
+      <c r="K4" s="1">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>AKHS_Mombasa</v>
@@ -756,8 +808,12 @@
       <c r="G5" s="3">
         <v>27079.67877</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -775,10 +831,22 @@
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>2024</v>
+      </c>
+      <c r="H7" s="1">
+        <v>2025</v>
+      </c>
+      <c r="I7" s="1">
+        <v>2026</v>
+      </c>
+      <c r="J7" s="1">
+        <v>2027</v>
+      </c>
+      <c r="K7" s="1">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>AKHS_Mombasa</v>
@@ -794,8 +862,12 @@
       <c r="G8" s="3">
         <v>5636.80524</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -813,10 +885,22 @@
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>2024</v>
+      </c>
+      <c r="H10" s="1">
+        <v>2025</v>
+      </c>
+      <c r="I10" s="1">
+        <v>2026</v>
+      </c>
+      <c r="J10" s="1">
+        <v>2027</v>
+      </c>
+      <c r="K10" s="1">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>AKHS_Mombasa</v>
@@ -832,8 +916,12 @@
       <c r="G11" s="3">
         <v>32266.70355972084</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
@@ -851,10 +939,22 @@
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>2024</v>
+      </c>
+      <c r="H13" s="1">
+        <v>2025</v>
+      </c>
+      <c r="I13" s="1">
+        <v>2026</v>
+      </c>
+      <c r="J13" s="1">
+        <v>2027</v>
+      </c>
+      <c r="K13" s="1">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>AKHS_Mombasa</v>
@@ -870,8 +970,12 @@
       <c r="G14" s="3">
         <v>23932.0312</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -889,10 +993,22 @@
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>2024</v>
+      </c>
+      <c r="H16" s="1">
+        <v>2025</v>
+      </c>
+      <c r="I16" s="1">
+        <v>2026</v>
+      </c>
+      <c r="J16" s="1">
+        <v>2027</v>
+      </c>
+      <c r="K16" s="1">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>AKHS_Mombasa</v>
@@ -908,8 +1024,12 @@
       <c r="G17" s="3">
         <v>64549.918875</v>
       </c>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -927,10 +1047,22 @@
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>2024</v>
+      </c>
+      <c r="H19" s="1">
+        <v>2025</v>
+      </c>
+      <c r="I19" s="1">
+        <v>2026</v>
+      </c>
+      <c r="J19" s="1">
+        <v>2027</v>
+      </c>
+      <c r="K19" s="1">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>AKHS_Mombasa</v>
@@ -946,8 +1078,12 @@
       <c r="G20" s="3">
         <v>129723.45024</v>
       </c>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -965,10 +1101,22 @@
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>2024</v>
+      </c>
+      <c r="H22" s="1">
+        <v>2025</v>
+      </c>
+      <c r="I22" s="1">
+        <v>2026</v>
+      </c>
+      <c r="J22" s="1">
+        <v>2027</v>
+      </c>
+      <c r="K22" s="1">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>AKHS_Mombasa</v>
@@ -984,70 +1132,74 @@
       <c r="G23" s="3">
         <v>27984.05230769231</v>
       </c>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E11">
     <cfRule type="expression" dxfId="0" priority="7">
-      <formula>COUNTIF(G11:G11,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(G11:K11,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="8">
-      <formula>AND(COUNTIF(G11:G11,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E11)))</formula>
+      <formula>AND(COUNTIF(G11:K11,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
     <cfRule type="expression" dxfId="0" priority="9">
-      <formula>COUNTIF(G14:G14,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(G14:K14,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="10">
-      <formula>AND(COUNTIF(G14:G14,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E14)))</formula>
+      <formula>AND(COUNTIF(G14:K14,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17">
     <cfRule type="expression" dxfId="0" priority="11">
-      <formula>COUNTIF(G17:G17,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(G17:K17,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="12">
-      <formula>AND(COUNTIF(G17:G17,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E17)))</formula>
+      <formula>AND(COUNTIF(G17:K17,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>COUNTIF(G2:G2,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(G2:K2,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="2">
-      <formula>AND(COUNTIF(G2:G2,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E2)))</formula>
+      <formula>AND(COUNTIF(G2:K2,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20">
     <cfRule type="expression" dxfId="0" priority="13">
-      <formula>COUNTIF(G20:G20,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(G20:K20,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="14">
-      <formula>AND(COUNTIF(G20:G20,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E20)))</formula>
+      <formula>AND(COUNTIF(G20:K20,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
     <cfRule type="expression" dxfId="0" priority="15">
-      <formula>COUNTIF(G23:G23,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(G23:K23,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="16">
-      <formula>AND(COUNTIF(G23:G23,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E23)))</formula>
+      <formula>AND(COUNTIF(G23:K23,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
     <cfRule type="expression" dxfId="0" priority="3">
-      <formula>COUNTIF(G5:G5,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(G5:K5,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="4">
-      <formula>AND(COUNTIF(G5:G5,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E5)))</formula>
+      <formula>AND(COUNTIF(G5:K5,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
     <cfRule type="expression" dxfId="0" priority="5">
-      <formula>COUNTIF(G8:G8,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(G8:K8,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="6">
-      <formula>AND(COUNTIF(G8:G8,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E8)))</formula>
+      <formula>AND(COUNTIF(G8:K8,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="8">
@@ -1085,7 +1237,7 @@
   <sheetPr>
     <tabColor rgb="FF808080"/>
   </sheetPr>
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1098,9 +1250,13 @@
     <col min="5" max="5" width="10.5703125" customWidth="1"/>
     <col min="6" max="6" width="3.85546875" customWidth="1"/>
     <col min="7" max="7" width="9.42578125" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -1118,10 +1274,22 @@
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>2024</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2025</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2026</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2027</v>
+      </c>
+      <c r="K1" s="1">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>AKHS_Mombasa</v>
@@ -1140,8 +1308,12 @@
         <v>12</v>
       </c>
       <c r="G2" s="3"/>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
@@ -1159,10 +1331,22 @@
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>2024</v>
+      </c>
+      <c r="H4" s="1">
+        <v>2025</v>
+      </c>
+      <c r="I4" s="1">
+        <v>2026</v>
+      </c>
+      <c r="J4" s="1">
+        <v>2027</v>
+      </c>
+      <c r="K4" s="1">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>AKHS_Mombasa</v>
@@ -1181,8 +1365,12 @@
         <v>12</v>
       </c>
       <c r="G5" s="3"/>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -1200,10 +1388,22 @@
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>2024</v>
+      </c>
+      <c r="H7" s="1">
+        <v>2025</v>
+      </c>
+      <c r="I7" s="1">
+        <v>2026</v>
+      </c>
+      <c r="J7" s="1">
+        <v>2027</v>
+      </c>
+      <c r="K7" s="1">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>AKHS_Mombasa</v>
@@ -1222,8 +1422,12 @@
         <v>12</v>
       </c>
       <c r="G8" s="3"/>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -1241,10 +1445,22 @@
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>2024</v>
+      </c>
+      <c r="H10" s="1">
+        <v>2025</v>
+      </c>
+      <c r="I10" s="1">
+        <v>2026</v>
+      </c>
+      <c r="J10" s="1">
+        <v>2027</v>
+      </c>
+      <c r="K10" s="1">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>AKHS_Mombasa</v>
@@ -1263,8 +1479,12 @@
         <v>12</v>
       </c>
       <c r="G11" s="3"/>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
@@ -1282,10 +1502,22 @@
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>2024</v>
+      </c>
+      <c r="H13" s="1">
+        <v>2025</v>
+      </c>
+      <c r="I13" s="1">
+        <v>2026</v>
+      </c>
+      <c r="J13" s="1">
+        <v>2027</v>
+      </c>
+      <c r="K13" s="1">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>AKHS_Mombasa</v>
@@ -1304,8 +1536,12 @@
         <v>12</v>
       </c>
       <c r="G14" s="3"/>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
@@ -1323,10 +1559,22 @@
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>2024</v>
+      </c>
+      <c r="H16" s="1">
+        <v>2025</v>
+      </c>
+      <c r="I16" s="1">
+        <v>2026</v>
+      </c>
+      <c r="J16" s="1">
+        <v>2027</v>
+      </c>
+      <c r="K16" s="1">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>AKHS_Mombasa</v>
@@ -1345,8 +1593,12 @@
         <v>12</v>
       </c>
       <c r="G17" s="3"/>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
@@ -1364,10 +1616,22 @@
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>2024</v>
+      </c>
+      <c r="H19" s="1">
+        <v>2025</v>
+      </c>
+      <c r="I19" s="1">
+        <v>2026</v>
+      </c>
+      <c r="J19" s="1">
+        <v>2027</v>
+      </c>
+      <c r="K19" s="1">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>AKHS_Mombasa</v>
@@ -1386,8 +1650,12 @@
         <v>12</v>
       </c>
       <c r="G20" s="3"/>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
@@ -1405,10 +1673,22 @@
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>2024</v>
+      </c>
+      <c r="H22" s="1">
+        <v>2025</v>
+      </c>
+      <c r="I22" s="1">
+        <v>2026</v>
+      </c>
+      <c r="J22" s="1">
+        <v>2027</v>
+      </c>
+      <c r="K22" s="1">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" s="1" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>AKHS_Mombasa</v>
@@ -1427,70 +1707,74 @@
         <v>12</v>
       </c>
       <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E11">
     <cfRule type="expression" dxfId="0" priority="7">
-      <formula>COUNTIF(G11:G11,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(G11:K11,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="8">
-      <formula>AND(COUNTIF(G11:G11,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E11)))</formula>
+      <formula>AND(COUNTIF(G11:K11,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
     <cfRule type="expression" dxfId="0" priority="9">
-      <formula>COUNTIF(G14:G14,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(G14:K14,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="10">
-      <formula>AND(COUNTIF(G14:G14,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E14)))</formula>
+      <formula>AND(COUNTIF(G14:K14,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17">
     <cfRule type="expression" dxfId="0" priority="11">
-      <formula>COUNTIF(G17:G17,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(G17:K17,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="12">
-      <formula>AND(COUNTIF(G17:G17,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E17)))</formula>
+      <formula>AND(COUNTIF(G17:K17,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>COUNTIF(G2:G2,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(G2:K2,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="2">
-      <formula>AND(COUNTIF(G2:G2,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E2)))</formula>
+      <formula>AND(COUNTIF(G2:K2,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20">
     <cfRule type="expression" dxfId="0" priority="13">
-      <formula>COUNTIF(G20:G20,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(G20:K20,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="14">
-      <formula>AND(COUNTIF(G20:G20,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E20)))</formula>
+      <formula>AND(COUNTIF(G20:K20,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
     <cfRule type="expression" dxfId="0" priority="15">
-      <formula>COUNTIF(G23:G23,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(G23:K23,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="16">
-      <formula>AND(COUNTIF(G23:G23,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E23)))</formula>
+      <formula>AND(COUNTIF(G23:K23,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
     <cfRule type="expression" dxfId="0" priority="3">
-      <formula>COUNTIF(G5:G5,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(G5:K5,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="4">
-      <formula>AND(COUNTIF(G5:G5,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E5)))</formula>
+      <formula>AND(COUNTIF(G5:K5,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
     <cfRule type="expression" dxfId="0" priority="5">
-      <formula>COUNTIF(G8:G8,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(G8:K8,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="6">
-      <formula>AND(COUNTIF(G8:G8,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E8)))</formula>
+      <formula>AND(COUNTIF(G8:K8,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(E8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="8">

</xml_diff>